<commit_message>
[DOC]Git_manual : Log 확인 및 SourceTree 등록 방법 추가
</commit_message>
<xml_diff>
--- a/Git_manual_20170404.xlsx
+++ b/Git_manual_20170404.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GitHub 가입" sheetId="13" r:id="rId1"/>
     <sheet name="GitHub Local 설정" sheetId="14" r:id="rId2"/>
+    <sheet name="Commit Log 확인 방법" sheetId="15" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Commit Log 확인 방법'!$A$1:$N$147</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'GitHub Local 설정'!$A$1:$L$320</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'GitHub 가입'!$A$1:$P$140</definedName>
   </definedNames>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>5. Repository 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,6 +180,42 @@
   </si>
   <si>
     <t>즉, Sync에서 Pull를 선택함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Commit history를 보고자하는 대상 폴더를 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Mouse Popup -&gt; TortoiseGit -&gt; Show log 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 아래와 같이 Log messages 창이 실행되며, Commit history가 보임</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Git Commit Log 보는 법 - TortoiseGit 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Git Commit Log 보는 법 - Source Tree 상용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Source Tree 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 탐색기에서 Clone 설정이 되어 있는 folder를 선택 및 drag하여 SourceTree의 탐색기 창에 추가한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 탐색기 창에 folder가 추가되고, 이를 선택하면, 아래와 같이 commit Log를 확인 할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 이후 SourceTree를 사용하여 Git 관리(commit, push, pull)가 가능한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2181,6 +2219,667 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>67408</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>55685</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>531681</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>84259</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="그룹 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="939312" y="905608"/>
+          <a:ext cx="6677504" cy="3853228"/>
+          <a:chOff x="910004" y="964224"/>
+          <a:chExt cx="6677504" cy="3853228"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="910004" y="964224"/>
+            <a:ext cx="6677504" cy="3853228"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3993173" y="1809750"/>
+            <a:ext cx="1033096" cy="215022"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4321420" y="4350727"/>
+            <a:ext cx="1033096" cy="215022"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5990493" y="3938954"/>
+            <a:ext cx="1321776" cy="215022"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>80597</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>432289</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>157515</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952501" y="5194789"/>
+          <a:ext cx="5876192" cy="4099399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>39972</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>58615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>168519</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>27293</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="911876" y="10895134"/>
+          <a:ext cx="4964316" cy="2943409"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>29308</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>73270</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>454269</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>141410</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="21" name="그룹 20"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="901212" y="14309482"/>
+          <a:ext cx="6638192" cy="5805120"/>
+          <a:chOff x="901212" y="14309482"/>
+          <a:chExt cx="6638192" cy="5805120"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="11" name="그림 10"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="901212" y="14309482"/>
+            <a:ext cx="4588849" cy="3011365"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="15" name="그림 14"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="3333750" y="16003064"/>
+            <a:ext cx="4205654" cy="4111538"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="모서리가 둥근 직사각형 16"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3209192" y="14961578"/>
+            <a:ext cx="1033096" cy="175845"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 17"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3383573" y="18564959"/>
+            <a:ext cx="1877158" cy="257906"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="20" name="직선 화살표 연결선 19"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3890596" y="15181385"/>
+            <a:ext cx="417635" cy="3348403"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>39437</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>51289</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>564174</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>47641</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="그룹 26"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="911341" y="21086885"/>
+          <a:ext cx="6737968" cy="3396044"/>
+          <a:chOff x="925994" y="21079557"/>
+          <a:chExt cx="6737968" cy="3396044"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="23" name="그림 22"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="925994" y="21079557"/>
+            <a:ext cx="6737968" cy="3396044"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="930519" y="23182384"/>
+            <a:ext cx="1677866" cy="257906"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="모서리가 둥근 직사각형 25"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3779226" y="24199361"/>
+            <a:ext cx="800101" cy="199293"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -2553,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D307"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A160" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="J205" sqref="J205"/>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="N179" sqref="N179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2726,4 +3425,71 @@
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H153" sqref="H153"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.25" customWidth="1"/>
+    <col min="2" max="5" width="4.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C118" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>